<commit_message>
Revisa especificação interface da remuneração
</commit_message>
<xml_diff>
--- a/espec002_remuneracao-servidores/static/leiaute_formularios_detalhamento.xlsx
+++ b/espec002_remuneracao-servidores/static/leiaute_formularios_detalhamento.xlsx
@@ -5,28 +5,29 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m752587\projects\especificacoes-portal-transparencia\espec002_remuneracao-servidores\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m13368964\Documents\Documents\CGE\Projetos-Transparencia-Ativa\especificacoes-portal-transparencia\espec002_remuneracao-servidores\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="722" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="722" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="24" r:id="rId1"/>
     <sheet name="situacao-funcional" sheetId="14" r:id="rId2"/>
     <sheet name="historico-recebimentos" sheetId="28" r:id="rId3"/>
-    <sheet name="formulario-detalhamento" sheetId="3" r:id="rId4"/>
-    <sheet name="historico" sheetId="17" r:id="rId5"/>
-    <sheet name="historico (3)" sheetId="26" r:id="rId6"/>
-    <sheet name="historico (4)" sheetId="27" r:id="rId7"/>
-    <sheet name="2.historico-remun-2015v2" sheetId="7" state="hidden" r:id="rId8"/>
+    <sheet name="formulario-detalhamento" sheetId="29" r:id="rId4"/>
+    <sheet name="formulario-detalhamento (1)" sheetId="3" r:id="rId5"/>
+    <sheet name="historico" sheetId="17" r:id="rId6"/>
+    <sheet name="historico (3)" sheetId="26" r:id="rId7"/>
+    <sheet name="historico (4)" sheetId="27" r:id="rId8"/>
+    <sheet name="2.historico-remun-2015v2" sheetId="7" state="hidden" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="161">
   <si>
     <t>Mês/Ano</t>
   </si>
@@ -493,6 +494,30 @@
   </si>
   <si>
     <t>Grat. Natalina</t>
+  </si>
+  <si>
+    <t>Vencimento Básico</t>
+  </si>
+  <si>
+    <t>Composição dos Jetons Empresas (R$)</t>
+  </si>
+  <si>
+    <t>Empresa 1</t>
+  </si>
+  <si>
+    <t>Empresa 2</t>
+  </si>
+  <si>
+    <t>Empresa 3</t>
+  </si>
+  <si>
+    <t>Vantagens (R$)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Composição da Remuneração </t>
+  </si>
+  <si>
+    <t>Descontos (R$)</t>
   </si>
 </sst>
 </file>
@@ -500,9 +525,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -594,6 +619,12 @@
     <font>
       <sz val="20"/>
       <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1564,9 +1595,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1601,34 +1632,34 @@
     <xf numFmtId="17" fontId="4" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="39" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="39" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="13" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="13" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="13" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="13" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1658,34 +1689,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1700,34 +1731,34 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1808,25 +1839,70 @@
     <xf numFmtId="17" fontId="4" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="4" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1876,6 +1952,15 @@
     </xf>
     <xf numFmtId="17" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1956,6 +2041,16 @@
     <cellStyle name="Vírgula" xfId="2" builtinId="3"/>
   </cellStyles>
   <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1972,16 +2067,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2136,15 +2221,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1371600</xdr:colOff>
+      <xdr:colOff>1026318</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
+      <xdr:rowOff>164306</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1562100</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1216818</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>404812</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2168,8 +2253,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2876550" y="1800225"/>
-          <a:ext cx="190500" cy="238125"/>
+          <a:off x="2526506" y="1676400"/>
+          <a:ext cx="190500" cy="240506"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2274,13 +2359,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>1381125</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
+      <xdr:rowOff>150019</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1571625</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2304,8 +2389,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7658100" y="1809750"/>
-          <a:ext cx="190500" cy="238125"/>
+          <a:off x="7667625" y="1662113"/>
+          <a:ext cx="190500" cy="240506"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2340,15 +2425,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:colOff>1107282</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
+      <xdr:rowOff>69056</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1297782</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>309562</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2372,8 +2457,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13125450" y="1800225"/>
-          <a:ext cx="190500" cy="238125"/>
+          <a:off x="13096876" y="1581150"/>
+          <a:ext cx="190500" cy="240506"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2408,15 +2493,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:colOff>904875</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
+      <xdr:rowOff>150019</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>1095375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2440,8 +2525,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9010650" y="1809750"/>
-          <a:ext cx="190500" cy="238125"/>
+          <a:off x="8786813" y="1662113"/>
+          <a:ext cx="190500" cy="240506"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2476,15 +2561,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:colOff>1157288</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1345407</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>269081</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2508,8 +2593,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10420350" y="1819275"/>
-          <a:ext cx="190500" cy="238125"/>
+          <a:off x="10408444" y="1540669"/>
+          <a:ext cx="188119" cy="240506"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2544,15 +2629,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1381125</xdr:colOff>
+      <xdr:colOff>1012032</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
+      <xdr:rowOff>164307</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1571625</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1202532</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>404813</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2576,8 +2661,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4476750" y="1800225"/>
-          <a:ext cx="190500" cy="238125"/>
+          <a:off x="4107657" y="1676401"/>
+          <a:ext cx="190500" cy="240506"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2612,15 +2697,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1390650</xdr:colOff>
+      <xdr:colOff>1271587</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
+      <xdr:rowOff>164307</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1581150</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1462087</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>404813</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2644,8 +2729,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6076950" y="1800225"/>
-          <a:ext cx="190500" cy="238125"/>
+          <a:off x="5962650" y="1676401"/>
+          <a:ext cx="190500" cy="240506"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2680,15 +2765,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:colOff>1035844</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>1226344</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>350043</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2712,8 +2797,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11753850" y="1828800"/>
-          <a:ext cx="190500" cy="238125"/>
+          <a:off x="11656219" y="1621631"/>
+          <a:ext cx="190500" cy="240506"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2749,6 +2834,232 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Multiplicar 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="219075"/>
+          <a:ext cx="0" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1876425</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2057400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Multiplicar 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7639050" y="219075"/>
+          <a:ext cx="0" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Multiplicar 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2609850"/>
+          <a:ext cx="0" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7277100" y="257175"/>
+          <a:ext cx="247650" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2974,7 +3285,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3523,7 +3834,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -4072,7 +4383,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -4621,7 +4932,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5579,7 +5890,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G37" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G37" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:G37"/>
   <sortState ref="A2:G37">
     <sortCondition ref="F2"/>
@@ -6795,7 +7106,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G37">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6813,8 +7124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6892,12 +7203,8 @@
       <c r="C7" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>38</v>
-      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -6911,7 +7218,7 @@
   <dimension ref="B1:J12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6926,54 +7233,54 @@
       <c r="B1" s="28"/>
     </row>
     <row r="2" spans="2:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
     </row>
     <row r="3" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95" t="s">
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="110" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="93"/>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="108"/>
+      <c r="C4" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="100" t="s">
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="102" t="s">
+      <c r="I4" s="117" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="96"/>
+      <c r="J4" s="111"/>
     </row>
     <row r="5" spans="2:10" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="94"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="82" t="s">
         <v>66</v>
       </c>
@@ -6989,9 +7296,9 @@
       <c r="G5" s="86" t="s">
         <v>151</v>
       </c>
-      <c r="H5" s="101"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="97"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="112"/>
     </row>
     <row r="6" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="55" t="s">
@@ -7000,7 +7307,7 @@
       <c r="C6" s="83">
         <v>16440.68</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="90">
         <v>0</v>
       </c>
       <c r="E6" s="39">
@@ -7032,7 +7339,7 @@
       <c r="C7" s="84">
         <v>16440.68</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="91">
         <v>0</v>
       </c>
       <c r="E7" s="34">
@@ -7063,7 +7370,7 @@
       <c r="C8" s="84">
         <v>16440.68</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="91">
         <v>0</v>
       </c>
       <c r="E8" s="34">
@@ -7094,7 +7401,7 @@
       <c r="C9" s="85">
         <v>12992.34</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="92">
         <v>0</v>
       </c>
       <c r="E9" s="35">
@@ -7152,10 +7459,325 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J47"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.5703125" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="124" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="126"/>
+    </row>
+    <row r="3" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="127" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="129"/>
+    </row>
+    <row r="4" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="121" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="123"/>
+    </row>
+    <row r="5" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="68"/>
+      <c r="C5" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="62">
+        <f>SUM(D6:D12)</f>
+        <v>18100.68</v>
+      </c>
+      <c r="E5" s="97"/>
+      <c r="F5" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="G5" s="69">
+        <f>SUM(G6:G9)</f>
+        <v>4833.04</v>
+      </c>
+      <c r="I5" s="66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="70"/>
+      <c r="C6" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="59">
+        <v>14811.42</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="71">
+        <v>1629.26</v>
+      </c>
+      <c r="I6" s="66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="70"/>
+      <c r="C7" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="71">
+        <v>3203.78</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="70"/>
+      <c r="C8" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="59"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="71"/>
+      <c r="I8" s="66" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="70"/>
+      <c r="C9" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="95">
+        <v>3289.26</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="71"/>
+    </row>
+    <row r="10" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="93"/>
+      <c r="C10" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="103"/>
+      <c r="G10" s="71"/>
+      <c r="I10" s="66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="93"/>
+      <c r="C11" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="95"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="71"/>
+      <c r="I11" s="66"/>
+    </row>
+    <row r="12" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="70"/>
+      <c r="C12" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="59"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="71"/>
+    </row>
+    <row r="13" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="121" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="123"/>
+    </row>
+    <row r="14" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="93"/>
+      <c r="C14" s="94" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="95">
+        <v>0</v>
+      </c>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="73"/>
+    </row>
+    <row r="15" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="96"/>
+      <c r="C15" s="94" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="95">
+        <v>0</v>
+      </c>
+      <c r="E15" s="102"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="74"/>
+    </row>
+    <row r="16" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="98"/>
+      <c r="C16" s="99" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="100">
+        <v>0</v>
+      </c>
+      <c r="E16" s="101"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+      <c r="J16" s="104"/>
+    </row>
+    <row r="17" spans="2:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+    </row>
+    <row r="18" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+    </row>
+    <row r="19" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="59"/>
+    </row>
+    <row r="43" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="59"/>
+    </row>
+    <row r="44" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="60"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="59"/>
+    </row>
+    <row r="45" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="60"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="60"/>
+    </row>
+    <row r="46" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+  </mergeCells>
+  <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
+  <pageSetup scale="79" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I45"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7171,36 +7793,36 @@
   <sheetData>
     <row r="1" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="108"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="126"/>
     </row>
     <row r="3" spans="2:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="111"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="129"/>
     </row>
     <row r="4" spans="2:9" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="130" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="113"/>
-      <c r="D4" s="113"/>
-      <c r="E4" s="113" t="s">
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="113"/>
-      <c r="G4" s="114"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="132"/>
       <c r="I4" s="66" t="s">
         <v>66</v>
       </c>
@@ -7505,7 +8127,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J11"/>
   <sheetViews>
@@ -7525,43 +8147,43 @@
       <c r="B1" s="28"/>
     </row>
     <row r="2" spans="2:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
     </row>
     <row r="3" spans="2:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="133" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="116" t="s">
+      <c r="C3" s="134" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="117" t="s">
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="135" t="s">
         <v>114</v>
       </c>
-      <c r="H3" s="115" t="s">
+      <c r="H3" s="133" t="s">
         <v>111</v>
       </c>
-      <c r="I3" s="115" t="s">
+      <c r="I3" s="133" t="s">
         <v>115</v>
       </c>
-      <c r="J3" s="120" t="s">
+      <c r="J3" s="138" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="4" spans="2:10" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="94"/>
+      <c r="B4" s="109"/>
       <c r="C4" s="41" t="s">
         <v>112</v>
       </c>
@@ -7574,221 +8196,10 @@
       <c r="F4" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="119"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="97"/>
-    </row>
-    <row r="5" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="50">
-        <v>16440.68</v>
-      </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47">
-        <f>2111+16440.68</f>
-        <v>18551.68</v>
-      </c>
-      <c r="G5" s="39">
-        <f>SUM(C5:F5)</f>
-        <v>34992.36</v>
-      </c>
-      <c r="H5" s="40">
-        <v>9666.08</v>
-      </c>
-      <c r="I5" s="40">
-        <f>G5-H5</f>
-        <v>25326.28</v>
-      </c>
-      <c r="J5" s="52">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="32">
-        <v>16440.68</v>
-      </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48">
-        <v>2506</v>
-      </c>
-      <c r="G6" s="34">
-        <f>SUM(C6:F6)</f>
-        <v>18946.68</v>
-      </c>
-      <c r="H6" s="36">
-        <v>5679.04</v>
-      </c>
-      <c r="I6" s="36">
-        <f>G6-H6</f>
-        <v>13267.64</v>
-      </c>
-      <c r="J6" s="53"/>
-    </row>
-    <row r="7" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="32">
-        <v>16440.68</v>
-      </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48">
-        <v>42599.99</v>
-      </c>
-      <c r="G7" s="34">
-        <f>SUM(C7:F7)</f>
-        <v>59040.67</v>
-      </c>
-      <c r="H7" s="36">
-        <v>10009.959999999999</v>
-      </c>
-      <c r="I7" s="36">
-        <f>G7-H7</f>
-        <v>49030.71</v>
-      </c>
-      <c r="J7" s="53">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="57" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="51">
-        <v>12992.34</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49">
-        <f>1318.19+4330.78</f>
-        <v>5648.9699999999993</v>
-      </c>
-      <c r="G8" s="35">
-        <f>SUM(C8:F8)</f>
-        <v>18641.309999999998</v>
-      </c>
-      <c r="H8" s="37">
-        <v>5243.77</v>
-      </c>
-      <c r="I8" s="37">
-        <f>G8-H8</f>
-        <v>13397.539999999997</v>
-      </c>
-      <c r="J8" s="54"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="45"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="64"/>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-  </mergeCells>
-  <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J11"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="6" width="23.85546875" customWidth="1"/>
-    <col min="7" max="10" width="20.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="28"/>
-    </row>
-    <row r="2" spans="2:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-    </row>
-    <row r="3" spans="2:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="115" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="116" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="117" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="115" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="115" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="120" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="94"/>
-      <c r="C4" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="81" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="119"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="97"/>
+      <c r="G4" s="137"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="112"/>
     </row>
     <row r="5" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="55" t="s">
@@ -7932,6 +8343,217 @@
   <dimension ref="B1:J11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="6" width="23.85546875" customWidth="1"/>
+    <col min="7" max="10" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="28"/>
+    </row>
+    <row r="2" spans="2:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="105" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+    </row>
+    <row r="3" spans="2:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="133" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="134" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="135" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="133" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="133" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="138" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="109"/>
+      <c r="C4" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="137"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="112"/>
+    </row>
+    <row r="5" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="50">
+        <v>16440.68</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47">
+        <f>2111+16440.68</f>
+        <v>18551.68</v>
+      </c>
+      <c r="G5" s="39">
+        <f>SUM(C5:F5)</f>
+        <v>34992.36</v>
+      </c>
+      <c r="H5" s="40">
+        <v>9666.08</v>
+      </c>
+      <c r="I5" s="40">
+        <f>G5-H5</f>
+        <v>25326.28</v>
+      </c>
+      <c r="J5" s="52">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="32">
+        <v>16440.68</v>
+      </c>
+      <c r="D6" s="34"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48">
+        <v>2506</v>
+      </c>
+      <c r="G6" s="34">
+        <f>SUM(C6:F6)</f>
+        <v>18946.68</v>
+      </c>
+      <c r="H6" s="36">
+        <v>5679.04</v>
+      </c>
+      <c r="I6" s="36">
+        <f>G6-H6</f>
+        <v>13267.64</v>
+      </c>
+      <c r="J6" s="53"/>
+    </row>
+    <row r="7" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="32">
+        <v>16440.68</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48">
+        <v>42599.99</v>
+      </c>
+      <c r="G7" s="34">
+        <f>SUM(C7:F7)</f>
+        <v>59040.67</v>
+      </c>
+      <c r="H7" s="36">
+        <v>10009.959999999999</v>
+      </c>
+      <c r="I7" s="36">
+        <f>G7-H7</f>
+        <v>49030.71</v>
+      </c>
+      <c r="J7" s="53">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="51">
+        <v>12992.34</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49">
+        <f>1318.19+4330.78</f>
+        <v>5648.9699999999993</v>
+      </c>
+      <c r="G8" s="35">
+        <f>SUM(C8:F8)</f>
+        <v>18641.309999999998</v>
+      </c>
+      <c r="H8" s="37">
+        <v>5243.77</v>
+      </c>
+      <c r="I8" s="37">
+        <f>G8-H8</f>
+        <v>13397.539999999997</v>
+      </c>
+      <c r="J8" s="54"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="44"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="45"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="64"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+  </mergeCells>
+  <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J3" sqref="J3:J4"/>
     </sheetView>
   </sheetViews>
@@ -7947,41 +8569,41 @@
       <c r="B1" s="28"/>
     </row>
     <row r="2" spans="2:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
     </row>
     <row r="3" spans="2:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="133" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="139" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="115" t="s">
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="135"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="115" t="s">
+      <c r="I3" s="133" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="120" t="s">
+      <c r="J3" s="138" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:10" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="94"/>
+      <c r="B4" s="109"/>
       <c r="C4" s="41" t="s">
         <v>66</v>
       </c>
@@ -7997,9 +8619,9 @@
       <c r="G4" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="97"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="112"/>
     </row>
     <row r="5" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="55" t="s">
@@ -8137,7 +8759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O8"/>
   <sheetViews>
@@ -8160,51 +8782,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="106"/>
+      <c r="O1" s="106"/>
     </row>
     <row r="2" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="124" t="s">
+      <c r="C2" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="122" t="s">
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="140" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="127" t="s">
+      <c r="K2" s="143"/>
+      <c r="L2" s="143"/>
+      <c r="M2" s="143"/>
+      <c r="N2" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="126" t="s">
+      <c r="O2" s="144" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="123"/>
+      <c r="B3" s="141"/>
       <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
@@ -8238,8 +8860,8 @@
       <c r="M3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="128"/>
-      <c r="O3" s="129"/>
+      <c r="N3" s="146"/>
+      <c r="O3" s="147"/>
     </row>
     <row r="4" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="26" t="s">

</xml_diff>